<commit_message>
Updates to ResponseVariables.XLSX files
</commit_message>
<xml_diff>
--- a/Data/ResponseVariables.xlsx
+++ b/Data/ResponseVariables.xlsx
@@ -9,21 +9,21 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25815" windowHeight="11670" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25815" windowHeight="11670"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="2" r:id="rId1"/>
     <sheet name="VariableRankings" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VariableRankings!$A$1:$K$92</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VariableRankings!$B$1:$L$92</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="226">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="228">
   <si>
     <t>variable</t>
   </si>
@@ -728,6 +728,12 @@
   </si>
   <si>
     <t>Direct impact from any action</t>
+  </si>
+  <si>
+    <t>id</t>
+  </si>
+  <si>
+    <t>Unique id assigned to each variable</t>
   </si>
 </sst>
 </file>
@@ -1305,7 +1311,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1330,6 +1336,9 @@
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1339,7 +1348,7 @@
     <xf numFmtId="0" fontId="16" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -1669,10 +1678,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1694,18 +1703,18 @@
       <c r="C1" s="4" t="s">
         <v>203</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>204</v>
       </c>
-      <c r="F1" s="16"/>
-      <c r="G1" s="16"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>0</v>
+        <v>226</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>199</v>
+        <v>227</v>
       </c>
       <c r="C2" s="6"/>
       <c r="E2" s="12" t="s">
@@ -1720,10 +1729,10 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="C3" s="6"/>
       <c r="E3" s="8" t="s">
@@ -1733,20 +1742,18 @@
         <v>0</v>
       </c>
       <c r="G3" s="10">
-        <f>COUNTIF(VariableRankings!K:K,F3)</f>
+        <f>COUNTIF(VariableRankings!L:L,F3)</f>
         <v>16</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A4" s="7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="C4" s="14" t="s">
-        <v>221</v>
-      </c>
+      <c r="A4" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>201</v>
+      </c>
+      <c r="C4" s="6"/>
       <c r="E4" s="8" t="s">
         <v>208</v>
       </c>
@@ -1754,18 +1761,20 @@
         <v>1</v>
       </c>
       <c r="G4" s="10">
-        <f>COUNTIF(VariableRankings!K:K,F4)</f>
+        <f>COUNTIF(VariableRankings!L:L,F4)</f>
         <v>17</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="C5" s="15"/>
+        <v>213</v>
+      </c>
+      <c r="C5" s="15" t="s">
+        <v>221</v>
+      </c>
       <c r="E5" s="8" t="s">
         <v>209</v>
       </c>
@@ -1773,18 +1782,18 @@
         <v>2</v>
       </c>
       <c r="G5" s="10">
-        <f>COUNTIF(VariableRankings!K:K,F5)</f>
+        <f>COUNTIF(VariableRankings!L:L,F5)</f>
         <v>13</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="C6" s="15"/>
+        <v>214</v>
+      </c>
+      <c r="C6" s="16"/>
       <c r="E6" s="8" t="s">
         <v>211</v>
       </c>
@@ -1792,18 +1801,18 @@
         <v>3</v>
       </c>
       <c r="G6" s="10">
-        <f>COUNTIF(VariableRankings!K:K,F6)</f>
+        <f>COUNTIF(VariableRankings!L:L,F6)</f>
         <v>0</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="C7" s="15"/>
+        <v>215</v>
+      </c>
+      <c r="C7" s="16"/>
       <c r="E7" s="8" t="s">
         <v>222</v>
       </c>
@@ -1811,18 +1820,18 @@
         <v>4</v>
       </c>
       <c r="G7" s="10">
-        <f>COUNTIF(VariableRankings!K:K,F7)</f>
+        <f>COUNTIF(VariableRankings!L:L,F7)</f>
         <v>10</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="C8" s="15"/>
+        <v>216</v>
+      </c>
+      <c r="C8" s="16"/>
       <c r="E8" s="8" t="s">
         <v>223</v>
       </c>
@@ -1830,18 +1839,18 @@
         <v>5</v>
       </c>
       <c r="G8" s="10">
-        <f>COUNTIF(VariableRankings!K:K,F8)</f>
+        <f>COUNTIF(VariableRankings!L:L,F8)</f>
         <v>10</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="C9" s="15"/>
+        <v>217</v>
+      </c>
+      <c r="C9" s="16"/>
       <c r="E9" s="8" t="s">
         <v>224</v>
       </c>
@@ -1849,18 +1858,18 @@
         <v>6</v>
       </c>
       <c r="G9" s="10">
-        <f>COUNTIF(VariableRankings!K:K,F9)</f>
+        <f>COUNTIF(VariableRankings!L:L,F9)</f>
         <v>12</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="C10" s="15"/>
+        <v>218</v>
+      </c>
+      <c r="C10" s="16"/>
       <c r="E10" s="8" t="s">
         <v>225</v>
       </c>
@@ -1868,40 +1877,49 @@
         <v>7</v>
       </c>
       <c r="G10" s="10">
-        <f>COUNTIF(VariableRankings!K:K,F10)</f>
+        <f>COUNTIF(VariableRankings!L:L,F10)</f>
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>219</v>
+      </c>
+      <c r="C11" s="16"/>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
-      <c r="B11" s="7" t="s">
+      <c r="B12" s="7" t="s">
         <v>220</v>
       </c>
-      <c r="C11" s="15"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+      <c r="C12" s="16"/>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
-      <c r="B12" s="8" t="s">
+      <c r="B13" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="C12" s="9" t="s">
+      <c r="C13" s="9" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="22" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C22" s="5"/>
+    <row r="23" spans="3:3" x14ac:dyDescent="0.25">
+      <c r="C23" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="C4:C11"/>
+    <mergeCell ref="C5:C12"/>
     <mergeCell ref="E1:G1"/>
   </mergeCells>
   <hyperlinks>
-    <hyperlink ref="C12" location="Metadata!G1" display="See table"/>
+    <hyperlink ref="C13" location="Metadata!G1" display="See table"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1910,62 +1928,68 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K92"/>
+  <dimension ref="A1:L92"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M13" sqref="M13"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="92.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="11" width="9.140625" style="2"/>
+    <col min="1" max="1" width="9.140625" style="2"/>
+    <col min="2" max="2" width="23.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="92.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="12" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A1" s="18" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="18" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="18" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="18" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="18" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="18" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="2" t="s">
+      <c r="L1" s="18" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A2" s="2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="C2" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C2" s="13"/>
       <c r="D2" s="13"/>
       <c r="E2" s="13"/>
       <c r="F2" s="13"/>
@@ -1973,18 +1997,21 @@
       <c r="H2" s="13"/>
       <c r="I2" s="13"/>
       <c r="J2" s="13"/>
-      <c r="K2" s="13">
+      <c r="K2" s="13"/>
+      <c r="L2" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A3" s="2">
+        <v>2</v>
+      </c>
+      <c r="B3" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="C3" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="C3" s="13"/>
       <c r="D3" s="13"/>
       <c r="E3" s="13"/>
       <c r="F3" s="13"/>
@@ -1992,18 +2019,21 @@
       <c r="H3" s="13"/>
       <c r="I3" s="13"/>
       <c r="J3" s="13"/>
-      <c r="K3" s="13">
+      <c r="K3" s="13"/>
+      <c r="L3" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A4" s="2">
+        <v>3</v>
+      </c>
+      <c r="B4" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="C4" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="C4" s="13"/>
       <c r="D4" s="13"/>
       <c r="E4" s="13"/>
       <c r="F4" s="13"/>
@@ -2011,18 +2041,21 @@
       <c r="H4" s="13"/>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
-      <c r="K4" s="13">
+      <c r="K4" s="13"/>
+      <c r="L4" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" s="2">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C5" s="13"/>
       <c r="D5" s="13"/>
       <c r="E5" s="13"/>
       <c r="F5" s="13"/>
@@ -2030,18 +2063,21 @@
       <c r="H5" s="13"/>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
-      <c r="K5" s="13">
+      <c r="K5" s="13"/>
+      <c r="L5" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" s="2">
+        <v>5</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="C6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="13"/>
       <c r="D6" s="13"/>
       <c r="E6" s="13"/>
       <c r="F6" s="13"/>
@@ -2049,18 +2085,21 @@
       <c r="H6" s="13"/>
       <c r="I6" s="13"/>
       <c r="J6" s="13"/>
-      <c r="K6" s="13">
+      <c r="K6" s="13"/>
+      <c r="L6" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" s="2">
+        <v>6</v>
+      </c>
+      <c r="B7" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="C7" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C7" s="13"/>
       <c r="D7" s="13"/>
       <c r="E7" s="13"/>
       <c r="F7" s="13"/>
@@ -2068,18 +2107,21 @@
       <c r="H7" s="13"/>
       <c r="I7" s="13"/>
       <c r="J7" s="13"/>
-      <c r="K7" s="13">
+      <c r="K7" s="13"/>
+      <c r="L7" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" s="2">
+        <v>7</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="C8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C8" s="13"/>
       <c r="D8" s="13"/>
       <c r="E8" s="13"/>
       <c r="F8" s="13"/>
@@ -2087,18 +2129,21 @@
       <c r="H8" s="13"/>
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
-      <c r="K8" s="13">
+      <c r="K8" s="13"/>
+      <c r="L8" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" s="2">
+        <v>8</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C9" s="13"/>
       <c r="D9" s="13"/>
       <c r="E9" s="13"/>
       <c r="F9" s="13"/>
@@ -2106,74 +2151,89 @@
       <c r="H9" s="13"/>
       <c r="I9" s="13"/>
       <c r="J9" s="13"/>
-      <c r="K9" s="13">
+      <c r="K9" s="13"/>
+      <c r="L9" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A10" s="2">
+        <v>9</v>
+      </c>
+      <c r="B10" t="s">
         <v>27</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>28</v>
       </c>
-      <c r="G10" s="2" t="s">
+      <c r="H10" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K10" s="2">
+      <c r="L10" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A11" s="2">
+        <v>10</v>
+      </c>
+      <c r="B11" t="s">
         <v>30</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>31</v>
       </c>
-      <c r="F11" s="2" t="s">
+      <c r="G11" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="2">
+      <c r="L11" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A12" s="2">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>32</v>
       </c>
-      <c r="B12" t="s">
+      <c r="C12" t="s">
         <v>33</v>
       </c>
-      <c r="G12" s="2" t="s">
+      <c r="H12" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K12" s="2">
+      <c r="L12" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A13" s="2">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
         <v>34</v>
       </c>
-      <c r="B13" t="s">
+      <c r="C13" t="s">
         <v>35</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="F13" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K13" s="2">
+      <c r="L13" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="3" t="s">
+    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2">
+        <v>13</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="C14" s="13"/>
       <c r="D14" s="13"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
@@ -2181,124 +2241,151 @@
       <c r="H14" s="13"/>
       <c r="I14" s="13"/>
       <c r="J14" s="13"/>
-      <c r="K14" s="13">
+      <c r="K14" s="13"/>
+      <c r="L14" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A15" s="2">
+        <v>14</v>
+      </c>
+      <c r="B15" t="s">
         <v>38</v>
       </c>
-      <c r="B15" t="s">
+      <c r="C15" t="s">
         <v>39</v>
       </c>
-      <c r="K15" s="2">
+      <c r="L15" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A16" s="2">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
         <v>40</v>
       </c>
-      <c r="B16" t="s">
+      <c r="C16" t="s">
         <v>41</v>
       </c>
-      <c r="K16" s="2">
+      <c r="L16" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A17" s="2">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
         <v>42</v>
       </c>
-      <c r="B17" t="s">
+      <c r="C17" t="s">
         <v>43</v>
       </c>
-      <c r="G17" s="2" t="s">
+      <c r="H17" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K17" s="2">
+      <c r="L17" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A18" s="2">
+        <v>17</v>
+      </c>
+      <c r="B18" t="s">
         <v>44</v>
       </c>
-      <c r="B18" t="s">
+      <c r="C18" t="s">
         <v>45</v>
       </c>
-      <c r="G18" s="2" t="s">
+      <c r="H18" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K18" s="2">
+      <c r="L18" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A19" s="2">
+        <v>18</v>
+      </c>
+      <c r="B19" t="s">
         <v>46</v>
       </c>
-      <c r="B19" t="s">
+      <c r="C19" t="s">
         <v>47</v>
       </c>
-      <c r="E19" s="2" t="s">
+      <c r="F19" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K19" s="2">
+      <c r="L19" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A20" s="2">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
         <v>48</v>
       </c>
-      <c r="B20" t="s">
+      <c r="C20" t="s">
         <v>49</v>
       </c>
-      <c r="E20" s="2" t="s">
+      <c r="F20" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K20" s="2">
+      <c r="L20" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A21" s="2">
+        <v>20</v>
+      </c>
+      <c r="B21" t="s">
         <v>50</v>
       </c>
-      <c r="B21" t="s">
+      <c r="C21" t="s">
         <v>51</v>
       </c>
-      <c r="E21" s="2" t="s">
+      <c r="F21" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K21" s="2">
+      <c r="L21" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A22" s="2">
+        <v>21</v>
+      </c>
+      <c r="B22" t="s">
         <v>52</v>
       </c>
-      <c r="B22" t="s">
+      <c r="C22" t="s">
         <v>53</v>
       </c>
-      <c r="E22" s="2" t="s">
+      <c r="F22" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K22" s="2">
+      <c r="L22" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
+    <row r="23" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="3" t="s">
+      <c r="C23" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="C23" s="13"/>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
       <c r="F23" s="13"/>
@@ -2306,18 +2393,21 @@
       <c r="H23" s="13"/>
       <c r="I23" s="13"/>
       <c r="J23" s="13"/>
-      <c r="K23" s="13">
+      <c r="K23" s="13"/>
+      <c r="L23" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="24" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="2">
+        <v>23</v>
+      </c>
+      <c r="B24" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="C24" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="13"/>
       <c r="D24" s="13"/>
       <c r="E24" s="13"/>
       <c r="F24" s="13"/>
@@ -2325,18 +2415,21 @@
       <c r="H24" s="13"/>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
-      <c r="K24" s="13">
+      <c r="K24" s="13"/>
+      <c r="L24" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
+    <row r="25" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="2">
+        <v>24</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="C25" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="C25" s="13"/>
       <c r="D25" s="13"/>
       <c r="E25" s="13"/>
       <c r="F25" s="13"/>
@@ -2344,18 +2437,21 @@
       <c r="H25" s="13"/>
       <c r="I25" s="13"/>
       <c r="J25" s="13"/>
-      <c r="K25" s="13">
+      <c r="K25" s="13"/>
+      <c r="L25" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="3" t="s">
+    <row r="26" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="2">
+        <v>25</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="C26" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="C26" s="13"/>
       <c r="D26" s="13"/>
       <c r="E26" s="13"/>
       <c r="F26" s="13"/>
@@ -2363,316 +2459,379 @@
       <c r="H26" s="13"/>
       <c r="I26" s="13"/>
       <c r="J26" s="13"/>
-      <c r="K26" s="13">
+      <c r="K26" s="13"/>
+      <c r="L26" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A27" s="2">
+        <v>26</v>
+      </c>
+      <c r="B27" t="s">
         <v>62</v>
       </c>
-      <c r="B27" t="s">
+      <c r="C27" t="s">
         <v>63</v>
       </c>
-      <c r="K27" s="2">
+      <c r="L27" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A28" s="2">
+        <v>27</v>
+      </c>
+      <c r="B28" t="s">
         <v>64</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>65</v>
       </c>
-      <c r="K28" s="2">
+      <c r="L28" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A29" s="2">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
         <v>66</v>
       </c>
-      <c r="B29" t="s">
+      <c r="C29" t="s">
         <v>67</v>
       </c>
-      <c r="K29" s="2">
+      <c r="L29" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A30" s="2">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
         <v>68</v>
       </c>
-      <c r="B30" t="s">
+      <c r="C30" t="s">
         <v>69</v>
       </c>
-      <c r="K30" s="2">
+      <c r="L30" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A31" s="2">
+        <v>30</v>
+      </c>
+      <c r="B31" t="s">
         <v>70</v>
       </c>
-      <c r="B31" t="s">
+      <c r="C31" t="s">
         <v>71</v>
       </c>
-      <c r="H31" s="17" t="s">
+      <c r="I31" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K31" s="2">
+      <c r="L31" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A32" s="2">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
         <v>73</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>74</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H32" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K32" s="2">
+      <c r="E32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L32" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A33" t="s">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A33" s="2">
+        <v>32</v>
+      </c>
+      <c r="B33" t="s">
         <v>76</v>
       </c>
-      <c r="B33" t="s">
+      <c r="C33" t="s">
         <v>77</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H33" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K33" s="2">
+      <c r="E33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L33" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A34" s="2">
+        <v>33</v>
+      </c>
+      <c r="B34" t="s">
         <v>78</v>
       </c>
-      <c r="B34" t="s">
+      <c r="C34" t="s">
         <v>79</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H34" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K34" s="2">
+      <c r="E34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L34" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A35" s="2">
+        <v>34</v>
+      </c>
+      <c r="B35" t="s">
         <v>80</v>
       </c>
-      <c r="B35" t="s">
+      <c r="C35" t="s">
         <v>81</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H35" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K35" s="2">
+      <c r="E35" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L35" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A36" s="2">
+        <v>35</v>
+      </c>
+      <c r="B36" t="s">
         <v>82</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C36" t="s">
         <v>83</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H36" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K36" s="2">
+      <c r="E36" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L36" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A37" s="2">
+        <v>36</v>
+      </c>
+      <c r="B37" t="s">
         <v>84</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C37" t="s">
         <v>85</v>
       </c>
-      <c r="D37" s="17" t="s">
+      <c r="E37" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="H37" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K37" s="2">
+      <c r="I37" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L37" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A38" s="2">
+        <v>37</v>
+      </c>
+      <c r="B38" t="s">
         <v>86</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C38" t="s">
         <v>87</v>
       </c>
-      <c r="K38" s="2">
+      <c r="L38" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A39" s="2">
+        <v>38</v>
+      </c>
+      <c r="B39" t="s">
         <v>88</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C39" t="s">
         <v>89</v>
       </c>
-      <c r="H39" s="17" t="s">
+      <c r="I39" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K39" s="2">
+      <c r="L39" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A40" s="2">
+        <v>39</v>
+      </c>
+      <c r="B40" t="s">
         <v>90</v>
       </c>
-      <c r="B40" t="s">
+      <c r="C40" t="s">
         <v>91</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H40" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K40" s="2">
+      <c r="E40" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L40" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A41" s="2">
+        <v>40</v>
+      </c>
+      <c r="B41" t="s">
         <v>92</v>
       </c>
-      <c r="B41" t="s">
+      <c r="C41" t="s">
         <v>93</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H41" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K41" s="2">
+      <c r="E41" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I41" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L41" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A42" s="2">
+        <v>41</v>
+      </c>
+      <c r="B42" t="s">
         <v>94</v>
       </c>
-      <c r="B42" t="s">
+      <c r="C42" t="s">
         <v>95</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H42" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K42" s="2">
+      <c r="E42" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I42" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L42" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A43" s="2">
+        <v>42</v>
+      </c>
+      <c r="B43" t="s">
         <v>96</v>
       </c>
-      <c r="B43" t="s">
+      <c r="C43" t="s">
         <v>97</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H43" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K43" s="2">
+      <c r="E43" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L43" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A44" s="2">
+        <v>43</v>
+      </c>
+      <c r="B44" t="s">
         <v>98</v>
       </c>
-      <c r="B44" t="s">
+      <c r="C44" t="s">
         <v>99</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H44" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K44" s="2">
+      <c r="E44" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L44" s="2">
         <v>5</v>
       </c>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A45" s="2">
+        <v>44</v>
+      </c>
+      <c r="B45" t="s">
         <v>100</v>
       </c>
-      <c r="B45" t="s">
+      <c r="C45" t="s">
         <v>101</v>
       </c>
-      <c r="D45" s="17" t="s">
+      <c r="E45" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="H45" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K45" s="2">
+      <c r="I45" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L45" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
+        <v>45</v>
+      </c>
+      <c r="B46" t="s">
         <v>102</v>
       </c>
-      <c r="B46" t="s">
+      <c r="C46" t="s">
         <v>103</v>
       </c>
-      <c r="K46" s="2">
+      <c r="L46" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
+    <row r="47" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
+        <v>46</v>
+      </c>
+      <c r="B47" s="3" t="s">
         <v>104</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="C47" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="C47" s="13"/>
       <c r="D47" s="13"/>
       <c r="E47" s="13"/>
       <c r="F47" s="13"/>
@@ -2680,29 +2839,35 @@
       <c r="H47" s="13"/>
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
-      <c r="K47" s="13">
+      <c r="K47" s="13"/>
+      <c r="L47" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A48" t="s">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
+        <v>47</v>
+      </c>
+      <c r="B48" t="s">
         <v>106</v>
       </c>
-      <c r="B48" t="s">
+      <c r="C48" t="s">
         <v>107</v>
       </c>
-      <c r="K48" s="2">
+      <c r="L48" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
+    <row r="49" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
+        <v>48</v>
+      </c>
+      <c r="B49" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="C49" s="3" t="s">
         <v>109</v>
       </c>
-      <c r="C49" s="13"/>
       <c r="D49" s="13"/>
       <c r="E49" s="13"/>
       <c r="F49" s="13"/>
@@ -2710,18 +2875,21 @@
       <c r="H49" s="13"/>
       <c r="I49" s="13"/>
       <c r="J49" s="13"/>
-      <c r="K49" s="13">
+      <c r="K49" s="13"/>
+      <c r="L49" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:11" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
+    <row r="50" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
+        <v>49</v>
+      </c>
+      <c r="B50" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="C50" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="C50" s="13"/>
       <c r="D50" s="13"/>
       <c r="E50" s="13"/>
       <c r="F50" s="13"/>
@@ -2729,674 +2897,802 @@
       <c r="H50" s="13"/>
       <c r="I50" s="13"/>
       <c r="J50" s="13"/>
-      <c r="K50" s="13">
+      <c r="K50" s="13"/>
+      <c r="L50" s="13">
         <v>0</v>
       </c>
     </row>
-    <row r="51" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
+        <v>50</v>
+      </c>
+      <c r="B51" t="s">
         <v>112</v>
       </c>
-      <c r="B51" t="s">
+      <c r="C51" t="s">
         <v>113</v>
       </c>
-      <c r="K51" s="2">
+      <c r="L51" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A52" s="2">
+        <v>51</v>
+      </c>
+      <c r="B52" t="s">
         <v>114</v>
       </c>
-      <c r="B52" t="s">
+      <c r="C52" t="s">
         <v>115</v>
       </c>
-      <c r="K52" s="2">
+      <c r="L52" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A53" s="2">
+        <v>52</v>
+      </c>
+      <c r="B53" t="s">
         <v>116</v>
       </c>
-      <c r="B53" t="s">
+      <c r="C53" t="s">
         <v>117</v>
       </c>
-      <c r="H53" s="17" t="s">
+      <c r="I53" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K53" s="2">
+      <c r="L53" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="54" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A54" t="s">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A54" s="2">
+        <v>53</v>
+      </c>
+      <c r="B54" t="s">
         <v>118</v>
       </c>
-      <c r="B54" t="s">
+      <c r="C54" t="s">
         <v>119</v>
       </c>
-      <c r="C54" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="D54" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H54" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K54" s="2">
+      <c r="E54" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L54" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="55" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A55" s="2">
+        <v>54</v>
+      </c>
+      <c r="B55" t="s">
         <v>120</v>
       </c>
-      <c r="B55" t="s">
+      <c r="C55" t="s">
         <v>121</v>
       </c>
-      <c r="C55" s="17" t="s">
+      <c r="D55" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H55" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K55" s="2">
+      <c r="E55" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I55" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L55" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="56" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A56" s="2">
+        <v>55</v>
+      </c>
+      <c r="B56" t="s">
         <v>122</v>
       </c>
-      <c r="B56" t="s">
+      <c r="C56" t="s">
         <v>123</v>
       </c>
-      <c r="C56" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="D56" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H56" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K56" s="2">
+      <c r="E56" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I56" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L56" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="57" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A57" s="2">
+        <v>56</v>
+      </c>
+      <c r="B57" t="s">
         <v>124</v>
       </c>
-      <c r="B57" t="s">
+      <c r="C57" t="s">
         <v>125</v>
       </c>
-      <c r="C57" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="D57" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H57" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K57" s="2">
+      <c r="E57" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I57" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L57" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="58" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A58" s="2">
+        <v>57</v>
+      </c>
+      <c r="B58" t="s">
         <v>126</v>
       </c>
-      <c r="B58" t="s">
+      <c r="C58" t="s">
         <v>127</v>
       </c>
-      <c r="C58" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="D58" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H58" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K58" s="2">
+      <c r="E58" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I58" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L58" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="59" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A59" s="2">
+        <v>58</v>
+      </c>
+      <c r="B59" t="s">
         <v>128</v>
       </c>
-      <c r="B59" t="s">
+      <c r="C59" t="s">
         <v>129</v>
       </c>
-      <c r="D59" s="17" t="s">
+      <c r="E59" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="H59" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K59" s="2">
+      <c r="I59" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L59" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="60" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A60" s="2">
+        <v>59</v>
+      </c>
+      <c r="B60" t="s">
         <v>130</v>
       </c>
-      <c r="B60" t="s">
+      <c r="C60" t="s">
         <v>131</v>
       </c>
-      <c r="K60" s="2">
+      <c r="L60" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A61" s="2">
+        <v>60</v>
+      </c>
+      <c r="B61" t="s">
         <v>132</v>
       </c>
-      <c r="B61" t="s">
+      <c r="C61" t="s">
         <v>133</v>
       </c>
-      <c r="H61" s="17" t="s">
+      <c r="I61" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K61" s="2">
+      <c r="L61" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A62" s="2">
+        <v>61</v>
+      </c>
+      <c r="B62" t="s">
         <v>134</v>
       </c>
-      <c r="B62" t="s">
+      <c r="C62" t="s">
         <v>135</v>
       </c>
-      <c r="C62" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="D62" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H62" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K62" s="2">
+      <c r="E62" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I62" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L62" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="63" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A63" s="2">
+        <v>62</v>
+      </c>
+      <c r="B63" t="s">
         <v>136</v>
       </c>
-      <c r="B63" t="s">
+      <c r="C63" t="s">
         <v>137</v>
       </c>
-      <c r="C63" s="17" t="s">
+      <c r="D63" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D63" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H63" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K63" s="2">
+      <c r="E63" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I63" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L63" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="64" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A64" t="s">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A64" s="2">
+        <v>63</v>
+      </c>
+      <c r="B64" t="s">
         <v>138</v>
       </c>
-      <c r="B64" t="s">
+      <c r="C64" t="s">
         <v>139</v>
       </c>
-      <c r="C64" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="D64" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H64" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K64" s="2">
+      <c r="E64" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I64" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L64" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="65" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A65" s="2">
+        <v>64</v>
+      </c>
+      <c r="B65" t="s">
         <v>140</v>
       </c>
-      <c r="B65" t="s">
+      <c r="C65" t="s">
         <v>141</v>
       </c>
-      <c r="C65" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="D65" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H65" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K65" s="2">
+      <c r="E65" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I65" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L65" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A66" s="2">
+        <v>65</v>
+      </c>
+      <c r="B66" t="s">
         <v>142</v>
       </c>
-      <c r="B66" t="s">
+      <c r="C66" t="s">
         <v>143</v>
       </c>
-      <c r="C66" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="D66" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H66" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K66" s="2">
+      <c r="E66" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I66" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L66" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="67" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A67" t="s">
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A67" s="2">
+        <v>66</v>
+      </c>
+      <c r="B67" t="s">
         <v>144</v>
       </c>
-      <c r="B67" t="s">
+      <c r="C67" t="s">
         <v>145</v>
       </c>
-      <c r="D67" s="17" t="s">
+      <c r="E67" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="H67" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K67" s="2">
+      <c r="I67" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L67" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="68" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A68" s="2">
+        <v>67</v>
+      </c>
+      <c r="B68" t="s">
         <v>146</v>
       </c>
-      <c r="B68" t="s">
+      <c r="C68" t="s">
         <v>147</v>
       </c>
-      <c r="K68" s="2">
+      <c r="L68" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A69" t="s">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A69" s="2">
+        <v>68</v>
+      </c>
+      <c r="B69" t="s">
         <v>148</v>
       </c>
-      <c r="B69" t="s">
+      <c r="C69" t="s">
         <v>149</v>
       </c>
-      <c r="H69" s="17" t="s">
+      <c r="I69" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="K69" s="2">
+      <c r="L69" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A70" s="2">
+        <v>69</v>
+      </c>
+      <c r="B70" t="s">
         <v>150</v>
       </c>
-      <c r="B70" t="s">
+      <c r="C70" t="s">
         <v>151</v>
       </c>
-      <c r="C70" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="D70" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H70" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K70" s="2">
+      <c r="E70" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I70" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L70" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A71" s="2">
+        <v>70</v>
+      </c>
+      <c r="B71" t="s">
         <v>152</v>
       </c>
-      <c r="B71" t="s">
+      <c r="C71" t="s">
         <v>153</v>
       </c>
-      <c r="C71" s="17" t="s">
+      <c r="D71" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="D71" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="H71" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K71" s="2">
+      <c r="E71" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I71" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L71" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="72" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A72" s="2">
+        <v>71</v>
+      </c>
+      <c r="B72" t="s">
         <v>154</v>
       </c>
-      <c r="B72" t="s">
+      <c r="C72" t="s">
         <v>155</v>
       </c>
-      <c r="C72" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="D72" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H72" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K72" s="2">
+      <c r="E72" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I72" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L72" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="73" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A73" t="s">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A73" s="2">
+        <v>72</v>
+      </c>
+      <c r="B73" t="s">
         <v>156</v>
       </c>
-      <c r="B73" t="s">
+      <c r="C73" t="s">
         <v>157</v>
       </c>
-      <c r="C73" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="D73" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H73" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K73" s="2">
+      <c r="E73" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I73" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L73" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="74" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A74" t="s">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A74" s="2">
+        <v>73</v>
+      </c>
+      <c r="B74" t="s">
         <v>158</v>
       </c>
-      <c r="B74" t="s">
+      <c r="C74" t="s">
         <v>159</v>
       </c>
-      <c r="C74" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="D74" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="H74" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K74" s="2">
+      <c r="E74" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I74" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L74" s="2">
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A75" t="s">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A75" s="2">
+        <v>74</v>
+      </c>
+      <c r="B75" t="s">
         <v>160</v>
       </c>
-      <c r="B75" t="s">
+      <c r="C75" t="s">
         <v>161</v>
       </c>
-      <c r="D75" s="17" t="s">
+      <c r="E75" s="14" t="s">
         <v>72</v>
       </c>
-      <c r="H75" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K75" s="2">
+      <c r="I75" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L75" s="2">
         <v>7</v>
       </c>
     </row>
-    <row r="76" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
         <v>162</v>
       </c>
-      <c r="B76" t="s">
+      <c r="C76" t="s">
         <v>163</v>
       </c>
-      <c r="C76" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K76" s="2">
+      <c r="D76" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L76" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="77" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
+        <v>76</v>
+      </c>
+      <c r="B77" t="s">
         <v>164</v>
       </c>
-      <c r="B77" t="s">
+      <c r="C77" t="s">
         <v>165</v>
       </c>
-      <c r="C77" s="2" t="s">
+      <c r="D77" s="2" t="s">
         <v>166</v>
       </c>
-      <c r="K77" s="2">
+      <c r="L77" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="78" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A78" s="2">
+        <v>77</v>
+      </c>
+      <c r="B78" t="s">
         <v>167</v>
       </c>
-      <c r="B78" t="s">
+      <c r="C78" t="s">
         <v>168</v>
       </c>
-      <c r="C78" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K78" s="2">
+      <c r="D78" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L78" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="79" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A79" s="2">
+        <v>78</v>
+      </c>
+      <c r="B79" t="s">
         <v>169</v>
       </c>
-      <c r="B79" t="s">
+      <c r="C79" t="s">
         <v>170</v>
       </c>
-      <c r="C79" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K79" s="2">
+      <c r="D79" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L79" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="80" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A80" s="2">
+        <v>79</v>
+      </c>
+      <c r="B80" t="s">
         <v>171</v>
       </c>
-      <c r="B80" t="s">
+      <c r="C80" t="s">
         <v>172</v>
       </c>
-      <c r="E80" s="2" t="s">
+      <c r="F80" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K80" s="2">
+      <c r="L80" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="81" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A81" s="2">
+        <v>80</v>
+      </c>
+      <c r="B81" t="s">
         <v>173</v>
       </c>
-      <c r="B81" t="s">
+      <c r="C81" t="s">
         <v>174</v>
       </c>
-      <c r="E81" s="2" t="s">
+      <c r="F81" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K81" s="2">
+      <c r="L81" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="82" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A82" s="2">
+        <v>81</v>
+      </c>
+      <c r="B82" t="s">
         <v>175</v>
       </c>
-      <c r="B82" t="s">
+      <c r="C82" t="s">
         <v>176</v>
       </c>
-      <c r="E82" s="2" t="s">
+      <c r="F82" s="2" t="s">
         <v>29</v>
       </c>
-      <c r="K82" s="2">
+      <c r="L82" s="2">
         <v>2</v>
       </c>
     </row>
-    <row r="83" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A83" s="2">
+        <v>82</v>
+      </c>
+      <c r="B83" t="s">
         <v>177</v>
       </c>
-      <c r="B83" t="s">
+      <c r="C83" t="s">
         <v>178</v>
       </c>
-      <c r="K83" s="2">
+      <c r="L83" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A84" s="2">
+        <v>83</v>
+      </c>
+      <c r="B84" t="s">
         <v>179</v>
       </c>
-      <c r="B84" t="s">
+      <c r="C84" t="s">
         <v>180</v>
       </c>
-      <c r="K84" s="2">
+      <c r="L84" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A85" s="2">
+        <v>84</v>
+      </c>
+      <c r="B85" t="s">
         <v>181</v>
       </c>
-      <c r="B85" t="s">
+      <c r="C85" t="s">
         <v>182</v>
       </c>
-      <c r="K85" s="2">
+      <c r="L85" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A86" s="2">
+        <v>85</v>
+      </c>
+      <c r="B86" t="s">
         <v>183</v>
       </c>
-      <c r="B86" t="s">
+      <c r="C86" t="s">
         <v>184</v>
       </c>
-      <c r="K86" s="2">
+      <c r="L86" s="2">
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A87" s="2">
+        <v>86</v>
+      </c>
+      <c r="B87" t="s">
         <v>185</v>
       </c>
-      <c r="B87" t="s">
+      <c r="C87" t="s">
         <v>186</v>
       </c>
-      <c r="J87" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K87" s="2">
+      <c r="K87" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L87" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="88" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A88" s="2">
+        <v>87</v>
+      </c>
+      <c r="B88" t="s">
         <v>187</v>
       </c>
-      <c r="B88" t="s">
+      <c r="C88" t="s">
         <v>188</v>
       </c>
-      <c r="J88" s="2" t="s">
+      <c r="K88" s="2" t="s">
         <v>189</v>
       </c>
-      <c r="K88" s="2">
+      <c r="L88" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="89" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A89" t="s">
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A89" s="2">
+        <v>88</v>
+      </c>
+      <c r="B89" t="s">
         <v>190</v>
       </c>
-      <c r="B89" t="s">
+      <c r="C89" t="s">
         <v>191</v>
       </c>
-      <c r="I89" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K89" s="2">
+      <c r="J89" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L89" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="90" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A90" s="2">
+        <v>89</v>
+      </c>
+      <c r="B90" t="s">
         <v>192</v>
       </c>
-      <c r="B90" t="s">
+      <c r="C90" t="s">
         <v>193</v>
       </c>
-      <c r="I90" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="K90" s="2">
+      <c r="J90" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L90" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="91" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A91" s="2">
+        <v>90</v>
+      </c>
+      <c r="B91" t="s">
         <v>194</v>
       </c>
-      <c r="B91" t="s">
+      <c r="C91" t="s">
         <v>195</v>
       </c>
-      <c r="D91" s="2" t="s">
+      <c r="E91" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="K91" s="2">
+      <c r="L91" s="2">
         <v>4</v>
       </c>
     </row>
-    <row r="92" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A92" s="2">
+        <v>91</v>
+      </c>
+      <c r="B92" t="s">
         <v>197</v>
       </c>
-      <c r="B92" t="s">
+      <c r="C92" t="s">
         <v>198</v>
       </c>
-      <c r="D92" s="2" t="s">
+      <c r="E92" s="2" t="s">
         <v>196</v>
       </c>
-      <c r="K92" s="2">
+      <c r="L92" s="2">
         <v>4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Re-ranked based on mtg.
</commit_message>
<xml_diff>
--- a/Data/ResponseVariables.xlsx
+++ b/Data/ResponseVariables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25815" windowHeight="11670"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9840" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="2" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="228">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="224">
   <si>
     <t>variable</t>
   </si>
@@ -592,9 +592,6 @@
     <t>Number of NPDES with catchment</t>
   </si>
   <si>
-    <t>?</t>
-  </si>
-  <si>
     <t>downstreamDistance_km</t>
   </si>
   <si>
@@ -649,16 +646,7 @@
     <t>Rank</t>
   </si>
   <si>
-    <t>No expected impact from any action</t>
-  </si>
-  <si>
-    <t>Indirect impact from 1 action</t>
-  </si>
-  <si>
     <t>Criteria</t>
-  </si>
-  <si>
-    <t>Indirect impact from &gt;1 actions</t>
   </si>
   <si>
     <t>Count</t>
@@ -718,29 +706,29 @@
     </r>
   </si>
   <si>
-    <t>Secondary impact from 1 action</t>
-  </si>
-  <si>
-    <t>Secondary impact from 2 actions</t>
-  </si>
-  <si>
-    <t>Secondary impact from &gt;2 actions</t>
-  </si>
-  <si>
-    <t>Direct impact from any action</t>
-  </si>
-  <si>
     <t>id</t>
   </si>
   <si>
     <t>Unique id assigned to each variable</t>
+  </si>
+  <si>
+    <t>Secondary impact from management</t>
+  </si>
+  <si>
+    <t>Direct impact, modeled in scenario</t>
+  </si>
+  <si>
+    <t>Direct impact, sensitivity evaluated</t>
+  </si>
+  <si>
+    <t>Original</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -904,6 +892,13 @@
       <u/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0" tint="-0.499984740745262"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1311,7 +1306,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1339,6 +1334,24 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1347,9 +1360,6 @@
     </xf>
     <xf numFmtId="0" fontId="16" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="43">
@@ -1680,8 +1690,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B22" sqref="B22"/>
+    <sheetView topLeftCell="B1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1691,40 +1701,41 @@
     <col min="3" max="3" width="50.85546875" customWidth="1"/>
     <col min="5" max="5" width="33.5703125" bestFit="1" customWidth="1"/>
     <col min="6" max="7" width="9.140625" style="2"/>
+    <col min="8" max="8" width="44.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
+        <v>202</v>
+      </c>
+      <c r="E1" s="25" t="s">
         <v>203</v>
       </c>
-      <c r="E1" s="17" t="s">
-        <v>204</v>
-      </c>
-      <c r="F1" s="17"/>
-      <c r="G1" s="17"/>
+      <c r="F1" s="25"/>
+      <c r="G1" s="25"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>226</v>
+        <v>218</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>227</v>
+        <v>219</v>
       </c>
       <c r="C2" s="6"/>
       <c r="E2" s="12" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1732,18 +1743,18 @@
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C3" s="6"/>
       <c r="E3" s="8" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="10">
         <f>COUNTIF(VariableRankings!L:L,F3)</f>
-        <v>16</v>
+        <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1751,18 +1762,18 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C4" s="6"/>
       <c r="E4" s="8" t="s">
-        <v>208</v>
+        <v>220</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
       </c>
       <c r="G4" s="10">
         <f>COUNTIF(VariableRankings!L:L,F4)</f>
-        <v>17</v>
+        <v>8</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1770,20 +1781,20 @@
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="C5" s="15" t="s">
-        <v>221</v>
+        <v>209</v>
+      </c>
+      <c r="C5" s="23" t="s">
+        <v>217</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>209</v>
+        <v>222</v>
       </c>
       <c r="F5" s="10">
         <v>2</v>
       </c>
       <c r="G5" s="10">
         <f>COUNTIF(VariableRankings!L:L,F5)</f>
-        <v>13</v>
+        <v>45</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
@@ -1791,18 +1802,18 @@
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="C6" s="16"/>
+        <v>210</v>
+      </c>
+      <c r="C6" s="24"/>
       <c r="E6" s="8" t="s">
-        <v>211</v>
+        <v>221</v>
       </c>
       <c r="F6" s="10">
         <v>3</v>
       </c>
       <c r="G6" s="10">
         <f>COUNTIF(VariableRankings!L:L,F6)</f>
-        <v>0</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
@@ -1810,104 +1821,64 @@
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="C7" s="16"/>
-      <c r="E7" s="8" t="s">
-        <v>222</v>
-      </c>
-      <c r="F7" s="10">
-        <v>4</v>
-      </c>
-      <c r="G7" s="10">
-        <f>COUNTIF(VariableRankings!L:L,F7)</f>
-        <v>10</v>
-      </c>
+        <v>211</v>
+      </c>
+      <c r="C7" s="24"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="C8" s="16"/>
-      <c r="E8" s="8" t="s">
-        <v>223</v>
-      </c>
-      <c r="F8" s="10">
-        <v>5</v>
-      </c>
-      <c r="G8" s="10">
-        <f>COUNTIF(VariableRankings!L:L,F8)</f>
-        <v>10</v>
-      </c>
+        <v>212</v>
+      </c>
+      <c r="C8" s="24"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>217</v>
-      </c>
-      <c r="C9" s="16"/>
-      <c r="E9" s="8" t="s">
-        <v>224</v>
-      </c>
-      <c r="F9" s="10">
-        <v>6</v>
-      </c>
-      <c r="G9" s="10">
-        <f>COUNTIF(VariableRankings!L:L,F9)</f>
-        <v>12</v>
-      </c>
+        <v>213</v>
+      </c>
+      <c r="C9" s="24"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>218</v>
-      </c>
-      <c r="C10" s="16"/>
-      <c r="E10" s="8" t="s">
-        <v>225</v>
-      </c>
-      <c r="F10" s="10">
-        <v>7</v>
-      </c>
-      <c r="G10" s="10">
-        <f>COUNTIF(VariableRankings!L:L,F10)</f>
-        <v>13</v>
-      </c>
+        <v>214</v>
+      </c>
+      <c r="C10" s="24"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>219</v>
-      </c>
-      <c r="C11" s="16"/>
+        <v>215</v>
+      </c>
+      <c r="C11" s="24"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>220</v>
-      </c>
-      <c r="C12" s="16"/>
+        <v>216</v>
+      </c>
+      <c r="C12" s="24"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
@@ -1928,10 +1899,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L92"/>
+  <dimension ref="A1:M92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O11" sqref="O11"/>
+    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
+      <selection activeCell="M92" sqref="M92"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1942,9 +1913,9 @@
     <col min="4" max="12" width="9.140625" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
-        <v>226</v>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
+        <v>218</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1952,35 +1923,38 @@
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="18" t="s">
-        <v>2</v>
-      </c>
-      <c r="E1" s="18" t="s">
+      <c r="D1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="F1" s="18" t="s">
+      <c r="F1" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="18" t="s">
+      <c r="H1" s="15" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="18" t="s">
+      <c r="I1" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="J1" s="18" t="s">
+      <c r="J1" s="15" t="s">
         <v>8</v>
       </c>
-      <c r="K1" s="18" t="s">
+      <c r="K1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="L1" s="18" t="s">
+      <c r="L1" s="15" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="15" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>1</v>
       </c>
@@ -2001,8 +1975,11 @@
       <c r="L2" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>2</v>
       </c>
@@ -2023,8 +2000,11 @@
       <c r="L3" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -2045,8 +2025,11 @@
       <c r="L4" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>4</v>
       </c>
@@ -2067,8 +2050,11 @@
       <c r="L5" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>5</v>
       </c>
@@ -2089,8 +2075,11 @@
       <c r="L6" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>6</v>
       </c>
@@ -2111,8 +2100,11 @@
       <c r="L7" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>7</v>
       </c>
@@ -2133,8 +2125,11 @@
       <c r="L8" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>8</v>
       </c>
@@ -2155,8 +2150,11 @@
       <c r="L9" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -2172,8 +2170,11 @@
       <c r="L10" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -2189,8 +2190,11 @@
       <c r="L11" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>11</v>
       </c>
@@ -2206,8 +2210,11 @@
       <c r="L12" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>12</v>
       </c>
@@ -2223,8 +2230,11 @@
       <c r="L13" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="14" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>13</v>
       </c>
@@ -2245,36 +2255,61 @@
       <c r="L14" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
+      <c r="M14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="16">
         <v>14</v>
       </c>
-      <c r="B15" t="s">
+      <c r="B15" s="17" t="s">
         <v>38</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C15" s="17" t="s">
         <v>39</v>
       </c>
-      <c r="L15" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="I15" s="16"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16">
+        <v>0</v>
+      </c>
+      <c r="M15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A16" s="16">
         <v>15</v>
       </c>
-      <c r="B16" t="s">
+      <c r="B16" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C16" s="17" t="s">
         <v>41</v>
       </c>
-      <c r="L16" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D16" s="16"/>
+      <c r="E16" s="16"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="16"/>
+      <c r="H16" s="16"/>
+      <c r="I16" s="16"/>
+      <c r="J16" s="16"/>
+      <c r="K16" s="16"/>
+      <c r="L16" s="16">
+        <v>0</v>
+      </c>
+      <c r="M16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>16</v>
       </c>
@@ -2290,8 +2325,11 @@
       <c r="L17" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>17</v>
       </c>
@@ -2307,8 +2345,11 @@
       <c r="L18" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>18</v>
       </c>
@@ -2324,8 +2365,11 @@
       <c r="L19" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -2341,8 +2385,11 @@
       <c r="L20" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>20</v>
       </c>
@@ -2358,8 +2405,11 @@
       <c r="L21" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>21</v>
       </c>
@@ -2375,8 +2425,11 @@
       <c r="L22" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>22</v>
       </c>
@@ -2397,8 +2450,11 @@
       <c r="L23" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -2419,8 +2475,11 @@
       <c r="L24" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -2441,8 +2500,11 @@
       <c r="L25" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="M25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>25</v>
       </c>
@@ -2463,8 +2525,11 @@
       <c r="L26" s="13">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>26</v>
       </c>
@@ -2477,8 +2542,11 @@
       <c r="L27" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>27</v>
       </c>
@@ -2491,8 +2559,11 @@
       <c r="L28" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>28</v>
       </c>
@@ -2505,8 +2576,11 @@
       <c r="L29" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2">
         <v>29</v>
       </c>
@@ -2519,8 +2593,11 @@
       <c r="L30" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M30">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2">
         <v>30</v>
       </c>
@@ -2530,14 +2607,20 @@
       <c r="C31" t="s">
         <v>71</v>
       </c>
+      <c r="E31" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="I31" s="14" t="s">
         <v>72</v>
       </c>
       <c r="L31" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="M31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2">
         <v>31</v>
       </c>
@@ -2554,10 +2637,13 @@
         <v>75</v>
       </c>
       <c r="L32" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M32">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -2574,10 +2660,13 @@
         <v>75</v>
       </c>
       <c r="L33" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M33">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -2594,10 +2683,13 @@
         <v>75</v>
       </c>
       <c r="L34" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M34">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -2614,10 +2706,13 @@
         <v>75</v>
       </c>
       <c r="L35" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M35">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -2634,10 +2729,13 @@
         <v>75</v>
       </c>
       <c r="L36" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M36">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -2654,10 +2752,13 @@
         <v>75</v>
       </c>
       <c r="L37" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="M37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -2670,8 +2771,11 @@
       <c r="L38" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -2681,14 +2785,20 @@
       <c r="C39" t="s">
         <v>89</v>
       </c>
+      <c r="E39" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="I39" s="14" t="s">
         <v>72</v>
       </c>
       <c r="L39" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="M39">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -2705,10 +2815,13 @@
         <v>75</v>
       </c>
       <c r="L40" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M40">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -2725,10 +2838,13 @@
         <v>75</v>
       </c>
       <c r="L41" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M41">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -2745,10 +2861,13 @@
         <v>75</v>
       </c>
       <c r="L42" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -2765,10 +2884,13 @@
         <v>75</v>
       </c>
       <c r="L43" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -2785,10 +2907,13 @@
         <v>75</v>
       </c>
       <c r="L44" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M44">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -2805,118 +2930,163 @@
         <v>75</v>
       </c>
       <c r="L45" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A46" s="2">
+        <v>3</v>
+      </c>
+      <c r="M45">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="18">
         <v>45</v>
       </c>
-      <c r="B46" t="s">
+      <c r="B46" s="19" t="s">
         <v>102</v>
       </c>
-      <c r="C46" t="s">
+      <c r="C46" s="19" t="s">
         <v>103</v>
       </c>
-      <c r="L46" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="2">
+      <c r="D46" s="18"/>
+      <c r="E46" s="18"/>
+      <c r="F46" s="18"/>
+      <c r="G46" s="18"/>
+      <c r="H46" s="18"/>
+      <c r="I46" s="18"/>
+      <c r="J46" s="18"/>
+      <c r="K46" s="18"/>
+      <c r="L46" s="18">
+        <v>0</v>
+      </c>
+      <c r="M46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A47" s="18">
         <v>46</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="20" t="s">
         <v>104</v>
       </c>
-      <c r="C47" s="3" t="s">
+      <c r="C47" s="20" t="s">
         <v>105</v>
       </c>
-      <c r="D47" s="13"/>
-      <c r="E47" s="13"/>
-      <c r="F47" s="13"/>
-      <c r="G47" s="13"/>
-      <c r="H47" s="13"/>
-      <c r="I47" s="13"/>
-      <c r="J47" s="13"/>
-      <c r="K47" s="13"/>
-      <c r="L47" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A48" s="2">
+      <c r="D47" s="21"/>
+      <c r="E47" s="21"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="21"/>
+      <c r="I47" s="21"/>
+      <c r="J47" s="21"/>
+      <c r="K47" s="21"/>
+      <c r="L47" s="21">
+        <v>0</v>
+      </c>
+      <c r="M47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A48" s="18">
         <v>47</v>
       </c>
-      <c r="B48" t="s">
+      <c r="B48" s="19" t="s">
         <v>106</v>
       </c>
-      <c r="C48" t="s">
+      <c r="C48" s="19" t="s">
         <v>107</v>
       </c>
-      <c r="L48" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="2">
+      <c r="D48" s="18"/>
+      <c r="E48" s="18"/>
+      <c r="F48" s="18"/>
+      <c r="G48" s="18"/>
+      <c r="H48" s="18"/>
+      <c r="I48" s="18"/>
+      <c r="J48" s="18"/>
+      <c r="K48" s="18"/>
+      <c r="L48" s="18">
+        <v>0</v>
+      </c>
+      <c r="M48">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="18">
         <v>48</v>
       </c>
-      <c r="B49" s="3" t="s">
+      <c r="B49" s="20" t="s">
         <v>108</v>
       </c>
-      <c r="C49" s="3" t="s">
+      <c r="C49" s="20" t="s">
         <v>109</v>
       </c>
-      <c r="D49" s="13"/>
-      <c r="E49" s="13"/>
-      <c r="F49" s="13"/>
-      <c r="G49" s="13"/>
-      <c r="H49" s="13"/>
-      <c r="I49" s="13"/>
-      <c r="J49" s="13"/>
-      <c r="K49" s="13"/>
-      <c r="L49" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="1:12" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="2">
+      <c r="D49" s="21"/>
+      <c r="E49" s="21"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="21"/>
+      <c r="I49" s="21"/>
+      <c r="J49" s="21"/>
+      <c r="K49" s="21"/>
+      <c r="L49" s="21">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="18">
         <v>49</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="20" t="s">
         <v>110</v>
       </c>
-      <c r="C50" s="3" t="s">
+      <c r="C50" s="20" t="s">
         <v>111</v>
       </c>
-      <c r="D50" s="13"/>
-      <c r="E50" s="13"/>
-      <c r="F50" s="13"/>
-      <c r="G50" s="13"/>
-      <c r="H50" s="13"/>
-      <c r="I50" s="13"/>
-      <c r="J50" s="13"/>
-      <c r="K50" s="13"/>
-      <c r="L50" s="13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A51" s="2">
+      <c r="D50" s="21"/>
+      <c r="E50" s="21"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="21"/>
+      <c r="I50" s="21"/>
+      <c r="J50" s="21"/>
+      <c r="K50" s="21"/>
+      <c r="L50" s="21">
+        <v>0</v>
+      </c>
+      <c r="M50">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="18">
         <v>50</v>
       </c>
-      <c r="B51" t="s">
+      <c r="B51" s="19" t="s">
         <v>112</v>
       </c>
-      <c r="C51" t="s">
+      <c r="C51" s="19" t="s">
         <v>113</v>
       </c>
-      <c r="L51" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D51" s="18"/>
+      <c r="E51" s="18"/>
+      <c r="F51" s="18"/>
+      <c r="G51" s="18"/>
+      <c r="H51" s="18"/>
+      <c r="I51" s="18"/>
+      <c r="J51" s="18"/>
+      <c r="K51" s="18"/>
+      <c r="L51" s="18">
+        <v>0</v>
+      </c>
+      <c r="M51">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -2929,8 +3099,11 @@
       <c r="L52" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2940,14 +3113,20 @@
       <c r="C53" t="s">
         <v>117</v>
       </c>
+      <c r="E53" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="I53" s="14" t="s">
         <v>72</v>
       </c>
       <c r="L53" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="M53">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2967,10 +3146,13 @@
         <v>75</v>
       </c>
       <c r="L54" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M54">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2990,10 +3172,13 @@
         <v>75</v>
       </c>
       <c r="L55" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="M55">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -3013,10 +3198,13 @@
         <v>75</v>
       </c>
       <c r="L56" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M56">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -3036,10 +3224,13 @@
         <v>75</v>
       </c>
       <c r="L57" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M57">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -3059,10 +3250,13 @@
         <v>75</v>
       </c>
       <c r="L58" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M58">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -3079,10 +3273,13 @@
         <v>75</v>
       </c>
       <c r="L59" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="M59">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -3095,8 +3292,11 @@
       <c r="L60" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M60">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -3110,10 +3310,13 @@
         <v>72</v>
       </c>
       <c r="L61" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="M61">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -3123,9 +3326,7 @@
       <c r="C62" t="s">
         <v>135</v>
       </c>
-      <c r="D62" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="D62" s="22"/>
       <c r="E62" s="2" t="s">
         <v>75</v>
       </c>
@@ -3133,10 +3334,13 @@
         <v>75</v>
       </c>
       <c r="L62" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M62">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -3146,9 +3350,7 @@
       <c r="C63" t="s">
         <v>137</v>
       </c>
-      <c r="D63" s="14" t="s">
-        <v>72</v>
-      </c>
+      <c r="D63" s="22"/>
       <c r="E63" s="2" t="s">
         <v>75</v>
       </c>
@@ -3156,10 +3358,13 @@
         <v>75</v>
       </c>
       <c r="L63" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M63">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>
@@ -3169,9 +3374,7 @@
       <c r="C64" t="s">
         <v>139</v>
       </c>
-      <c r="D64" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="D64" s="22"/>
       <c r="E64" s="2" t="s">
         <v>75</v>
       </c>
@@ -3179,10 +3382,13 @@
         <v>75</v>
       </c>
       <c r="L64" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M64">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65" s="2">
         <v>64</v>
       </c>
@@ -3192,9 +3398,7 @@
       <c r="C65" t="s">
         <v>141</v>
       </c>
-      <c r="D65" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="D65" s="22"/>
       <c r="E65" s="2" t="s">
         <v>75</v>
       </c>
@@ -3202,10 +3406,13 @@
         <v>75</v>
       </c>
       <c r="L65" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M65">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66" s="2">
         <v>65</v>
       </c>
@@ -3215,9 +3422,7 @@
       <c r="C66" t="s">
         <v>143</v>
       </c>
-      <c r="D66" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="D66" s="22"/>
       <c r="E66" s="2" t="s">
         <v>75</v>
       </c>
@@ -3225,10 +3430,13 @@
         <v>75</v>
       </c>
       <c r="L66" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M66">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67" s="2">
         <v>66</v>
       </c>
@@ -3238,6 +3446,7 @@
       <c r="C67" t="s">
         <v>145</v>
       </c>
+      <c r="D67" s="22"/>
       <c r="E67" s="14" t="s">
         <v>72</v>
       </c>
@@ -3245,10 +3454,13 @@
         <v>75</v>
       </c>
       <c r="L67" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="M67">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68" s="2">
         <v>67</v>
       </c>
@@ -3258,11 +3470,15 @@
       <c r="C68" t="s">
         <v>147</v>
       </c>
+      <c r="D68" s="22"/>
       <c r="L68" s="2">
         <v>1</v>
       </c>
-    </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69" s="2">
         <v>68</v>
       </c>
@@ -3272,14 +3488,18 @@
       <c r="C69" t="s">
         <v>149</v>
       </c>
+      <c r="D69" s="22"/>
       <c r="I69" s="14" t="s">
         <v>72</v>
       </c>
       <c r="L69" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="M69">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70" s="2">
         <v>69</v>
       </c>
@@ -3289,9 +3509,7 @@
       <c r="C70" t="s">
         <v>151</v>
       </c>
-      <c r="D70" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="D70" s="22"/>
       <c r="E70" s="2" t="s">
         <v>75</v>
       </c>
@@ -3299,10 +3517,13 @@
         <v>75</v>
       </c>
       <c r="L70" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M70">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71" s="2">
         <v>70</v>
       </c>
@@ -3312,9 +3533,7 @@
       <c r="C71" t="s">
         <v>153</v>
       </c>
-      <c r="D71" s="14" t="s">
-        <v>72</v>
-      </c>
+      <c r="D71" s="22"/>
       <c r="E71" s="2" t="s">
         <v>75</v>
       </c>
@@ -3322,10 +3541,13 @@
         <v>75</v>
       </c>
       <c r="L71" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M71">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72" s="2">
         <v>71</v>
       </c>
@@ -3335,9 +3557,7 @@
       <c r="C72" t="s">
         <v>155</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="D72" s="22"/>
       <c r="E72" s="2" t="s">
         <v>75</v>
       </c>
@@ -3345,10 +3565,13 @@
         <v>75</v>
       </c>
       <c r="L72" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M72">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73" s="2">
         <v>72</v>
       </c>
@@ -3358,9 +3581,7 @@
       <c r="C73" t="s">
         <v>157</v>
       </c>
-      <c r="D73" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="D73" s="22"/>
       <c r="E73" s="2" t="s">
         <v>75</v>
       </c>
@@ -3368,10 +3589,13 @@
         <v>75</v>
       </c>
       <c r="L73" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M73">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74" s="2">
         <v>73</v>
       </c>
@@ -3381,9 +3605,7 @@
       <c r="C74" t="s">
         <v>159</v>
       </c>
-      <c r="D74" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="D74" s="22"/>
       <c r="E74" s="2" t="s">
         <v>75</v>
       </c>
@@ -3391,10 +3613,13 @@
         <v>75</v>
       </c>
       <c r="L74" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M74">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75" s="2">
         <v>74</v>
       </c>
@@ -3404,6 +3629,7 @@
       <c r="C75" t="s">
         <v>161</v>
       </c>
+      <c r="D75" s="22"/>
       <c r="E75" s="14" t="s">
         <v>72</v>
       </c>
@@ -3411,44 +3637,67 @@
         <v>75</v>
       </c>
       <c r="L75" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A76" s="2">
-        <v>75</v>
-      </c>
-      <c r="B76" t="s">
+        <v>3</v>
+      </c>
+      <c r="M75">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="18">
+        <v>75</v>
+      </c>
+      <c r="B76" s="19" t="s">
         <v>162</v>
       </c>
-      <c r="C76" t="s">
+      <c r="C76" s="19" t="s">
         <v>163</v>
       </c>
-      <c r="D76" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L76" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A77" s="2">
+      <c r="D76" s="18" t="s">
+        <v>75</v>
+      </c>
+      <c r="E76" s="18"/>
+      <c r="F76" s="18"/>
+      <c r="G76" s="18"/>
+      <c r="H76" s="18"/>
+      <c r="I76" s="18"/>
+      <c r="J76" s="18"/>
+      <c r="K76" s="18"/>
+      <c r="L76" s="18">
+        <v>0</v>
+      </c>
+      <c r="M76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="18">
         <v>76</v>
       </c>
-      <c r="B77" t="s">
+      <c r="B77" s="19" t="s">
         <v>164</v>
       </c>
-      <c r="C77" t="s">
+      <c r="C77" s="19" t="s">
         <v>165</v>
       </c>
-      <c r="D77" s="2" t="s">
+      <c r="D77" s="18" t="s">
         <v>166</v>
       </c>
-      <c r="L77" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E77" s="18"/>
+      <c r="F77" s="18"/>
+      <c r="G77" s="18"/>
+      <c r="H77" s="18"/>
+      <c r="I77" s="18"/>
+      <c r="J77" s="18"/>
+      <c r="K77" s="18"/>
+      <c r="L77" s="18">
+        <v>0</v>
+      </c>
+      <c r="M77">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78" s="2">
         <v>77</v>
       </c>
@@ -3462,10 +3711,13 @@
         <v>75</v>
       </c>
       <c r="L78" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M78">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79" s="2">
         <v>78</v>
       </c>
@@ -3479,10 +3731,13 @@
         <v>75</v>
       </c>
       <c r="L79" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M79">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -3498,8 +3753,11 @@
       <c r="L80" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M80">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81" s="2">
         <v>80</v>
       </c>
@@ -3515,8 +3773,11 @@
       <c r="L81" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M81">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82" s="2">
         <v>81</v>
       </c>
@@ -3532,36 +3793,61 @@
       <c r="L82" s="2">
         <v>2</v>
       </c>
-    </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A83" s="2">
+      <c r="M82">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="16">
         <v>82</v>
       </c>
-      <c r="B83" t="s">
+      <c r="B83" s="17" t="s">
         <v>177</v>
       </c>
-      <c r="C83" t="s">
+      <c r="C83" s="17" t="s">
         <v>178</v>
       </c>
-      <c r="L83" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A84" s="2">
+      <c r="D83" s="16"/>
+      <c r="E83" s="16"/>
+      <c r="F83" s="16"/>
+      <c r="G83" s="16"/>
+      <c r="H83" s="16"/>
+      <c r="I83" s="16"/>
+      <c r="J83" s="16"/>
+      <c r="K83" s="16"/>
+      <c r="L83" s="16">
+        <v>0</v>
+      </c>
+      <c r="M83">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="84" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="18">
         <v>83</v>
       </c>
-      <c r="B84" t="s">
+      <c r="B84" s="19" t="s">
         <v>179</v>
       </c>
-      <c r="C84" t="s">
+      <c r="C84" s="19" t="s">
         <v>180</v>
       </c>
-      <c r="L84" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="D84" s="18"/>
+      <c r="E84" s="18"/>
+      <c r="F84" s="18"/>
+      <c r="G84" s="18"/>
+      <c r="H84" s="18"/>
+      <c r="I84" s="18"/>
+      <c r="J84" s="18"/>
+      <c r="K84" s="18"/>
+      <c r="L84" s="18">
+        <v>0</v>
+      </c>
+      <c r="M84">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85" s="2">
         <v>84</v>
       </c>
@@ -3572,10 +3858,13 @@
         <v>182</v>
       </c>
       <c r="L85" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M85">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86" s="2">
         <v>85</v>
       </c>
@@ -3586,10 +3875,13 @@
         <v>184</v>
       </c>
       <c r="L86" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M86">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87" s="2">
         <v>86</v>
       </c>
@@ -3603,10 +3895,13 @@
         <v>75</v>
       </c>
       <c r="L87" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M87">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88" s="2">
         <v>87</v>
       </c>
@@ -3617,78 +3912,107 @@
         <v>188</v>
       </c>
       <c r="K88" s="2" t="s">
-        <v>189</v>
+        <v>75</v>
       </c>
       <c r="L88" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M88">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89" s="2">
         <v>88</v>
       </c>
       <c r="B89" t="s">
+        <v>189</v>
+      </c>
+      <c r="C89" t="s">
         <v>190</v>
       </c>
-      <c r="C89" t="s">
-        <v>191</v>
-      </c>
       <c r="J89" s="2" t="s">
         <v>75</v>
       </c>
       <c r="L89" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="M89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90" s="2">
         <v>89</v>
       </c>
       <c r="B90" t="s">
+        <v>191</v>
+      </c>
+      <c r="C90" t="s">
         <v>192</v>
       </c>
-      <c r="C90" t="s">
+      <c r="J90" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L90" s="2">
+        <v>2</v>
+      </c>
+      <c r="M90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A91" s="16">
+        <v>90</v>
+      </c>
+      <c r="B91" s="17" t="s">
         <v>193</v>
       </c>
-      <c r="J90" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L90" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A91" s="2">
-        <v>90</v>
-      </c>
-      <c r="B91" t="s">
+      <c r="C91" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="C91" t="s">
+      <c r="D91" s="16"/>
+      <c r="E91" s="16" t="s">
         <v>195</v>
       </c>
-      <c r="E91" s="2" t="s">
+      <c r="F91" s="16"/>
+      <c r="G91" s="16"/>
+      <c r="H91" s="16"/>
+      <c r="I91" s="16"/>
+      <c r="J91" s="16"/>
+      <c r="K91" s="16"/>
+      <c r="L91" s="16">
+        <v>0</v>
+      </c>
+      <c r="M91">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="92" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A92" s="16">
+        <v>91</v>
+      </c>
+      <c r="B92" s="17" t="s">
         <v>196</v>
       </c>
-      <c r="L91" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
-      <c r="A92" s="2">
-        <v>91</v>
-      </c>
-      <c r="B92" t="s">
+      <c r="C92" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="C92" t="s">
-        <v>198</v>
-      </c>
-      <c r="E92" s="2" t="s">
-        <v>196</v>
-      </c>
-      <c r="L92" s="2">
-        <v>4</v>
+      <c r="D92" s="16"/>
+      <c r="E92" s="16" t="s">
+        <v>195</v>
+      </c>
+      <c r="F92" s="16"/>
+      <c r="G92" s="16"/>
+      <c r="H92" s="16"/>
+      <c r="I92" s="16"/>
+      <c r="J92" s="16"/>
+      <c r="K92" s="16"/>
+      <c r="L92" s="16">
+        <v>0</v>
+      </c>
+      <c r="M92">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Removed ESRI, Xings, Shadestats, Totlength
</commit_message>
<xml_diff>
--- a/Data/ResponseVariables.xlsx
+++ b/Data/ResponseVariables.xlsx
@@ -14,16 +14,17 @@
   <sheets>
     <sheet name="Metadata" sheetId="2" r:id="rId1"/>
     <sheet name="VariableRankings" sheetId="1" r:id="rId2"/>
+    <sheet name="Notes" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VariableRankings!$B$1:$L$92</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">VariableRankings!$B$1:$L$82</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="224">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="207">
   <si>
     <t>variable</t>
   </si>
@@ -331,42 +332,6 @@
     <t>Catchment area (km2) classified as wetland</t>
   </si>
   <si>
-    <t>flooding_SUM</t>
-  </si>
-  <si>
-    <t>Sum of flooding frequency values within a catchment</t>
-  </si>
-  <si>
-    <t>slope_MEAN</t>
-  </si>
-  <si>
-    <t>Mean slope (degrees)</t>
-  </si>
-  <si>
-    <t>road_density_MEAN</t>
-  </si>
-  <si>
-    <t>Sum of road length w/in 1km cells, averaged across all cells w/in a catchment</t>
-  </si>
-  <si>
-    <t>water_table_MEAN</t>
-  </si>
-  <si>
-    <t>Mean depth to water table (cm)</t>
-  </si>
-  <si>
-    <t>erodability_MEAN</t>
-  </si>
-  <si>
-    <t>Mean SSURGO Erodibility (K-factor) value</t>
-  </si>
-  <si>
-    <t>flood_risk_SUM</t>
-  </si>
-  <si>
-    <t>Proportion of catchment area in flood risk zone</t>
-  </si>
-  <si>
     <t>FLNLCD_1</t>
   </si>
   <si>
@@ -511,21 +476,6 @@
     <t>Percent of riparian zone classified as wetland</t>
   </si>
   <si>
-    <t>ShadedSegments</t>
-  </si>
-  <si>
-    <t>Number of flowline segments classified as shaded</t>
-  </si>
-  <si>
-    <t>ShadedLength</t>
-  </si>
-  <si>
-    <t>Total flowline length (m) intersecting NLCD (2011) forest</t>
-  </si>
-  <si>
-    <t>m-up (how is this one different)</t>
-  </si>
-  <si>
     <t>LongestSegment</t>
   </si>
   <si>
@@ -554,18 +504,6 @@
   </si>
   <si>
     <t>Percent of stream classified as warm</t>
-  </si>
-  <si>
-    <t>TotLength</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Total stream length (m) </t>
-  </si>
-  <si>
-    <t>Crossings</t>
-  </si>
-  <si>
-    <t>Count of road crossings found within the catchment</t>
   </si>
   <si>
     <t>PctCanopy</t>
@@ -722,6 +660,18 @@
   </si>
   <si>
     <t>Original</t>
+  </si>
+  <si>
+    <t>Deleted ESRI landscape stats</t>
+  </si>
+  <si>
+    <t>Deleted Road crosssings</t>
+  </si>
+  <si>
+    <t>Removed ShadedSegments and ShadedLength</t>
+  </si>
+  <si>
+    <t>Removed TotLength</t>
   </si>
 </sst>
 </file>
@@ -1306,7 +1256,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -1341,14 +1291,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1361,6 +1303,7 @@
     <xf numFmtId="0" fontId="16" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1706,36 +1649,36 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>199</v>
+        <v>178</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>202</v>
-      </c>
-      <c r="E1" s="25" t="s">
-        <v>203</v>
-      </c>
-      <c r="F1" s="25"/>
-      <c r="G1" s="25"/>
+        <v>181</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>182</v>
+      </c>
+      <c r="F1" s="21"/>
+      <c r="G1" s="21"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>219</v>
+        <v>198</v>
       </c>
       <c r="C2" s="6"/>
       <c r="E2" s="12" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>206</v>
+        <v>185</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>208</v>
+        <v>187</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1743,18 +1686,18 @@
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>198</v>
+        <v>177</v>
       </c>
       <c r="C3" s="6"/>
       <c r="E3" s="8" t="s">
-        <v>204</v>
+        <v>183</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="10">
         <f>COUNTIF(VariableRankings!L:L,F3)</f>
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1762,11 +1705,11 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>200</v>
+        <v>179</v>
       </c>
       <c r="C4" s="6"/>
       <c r="E4" s="8" t="s">
-        <v>220</v>
+        <v>199</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
@@ -1781,13 +1724,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>209</v>
-      </c>
-      <c r="C5" s="23" t="s">
-        <v>217</v>
+        <v>188</v>
+      </c>
+      <c r="C5" s="19" t="s">
+        <v>196</v>
       </c>
       <c r="E5" s="8" t="s">
-        <v>222</v>
+        <v>201</v>
       </c>
       <c r="F5" s="10">
         <v>2</v>
@@ -1802,11 +1745,11 @@
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>210</v>
-      </c>
-      <c r="C6" s="24"/>
+        <v>189</v>
+      </c>
+      <c r="C6" s="20"/>
       <c r="E6" s="8" t="s">
-        <v>221</v>
+        <v>200</v>
       </c>
       <c r="F6" s="10">
         <v>3</v>
@@ -1821,64 +1764,64 @@
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>211</v>
-      </c>
-      <c r="C7" s="24"/>
+        <v>190</v>
+      </c>
+      <c r="C7" s="20"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>212</v>
-      </c>
-      <c r="C8" s="24"/>
+        <v>191</v>
+      </c>
+      <c r="C8" s="20"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>213</v>
-      </c>
-      <c r="C9" s="24"/>
+        <v>192</v>
+      </c>
+      <c r="C9" s="20"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>214</v>
-      </c>
-      <c r="C10" s="24"/>
+        <v>193</v>
+      </c>
+      <c r="C10" s="20"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>215</v>
-      </c>
-      <c r="C11" s="24"/>
+        <v>194</v>
+      </c>
+      <c r="C11" s="20"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>216</v>
-      </c>
-      <c r="C12" s="24"/>
+        <v>195</v>
+      </c>
+      <c r="C12" s="20"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>201</v>
+        <v>180</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>205</v>
+        <v>184</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
@@ -1899,10 +1842,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M92"/>
+  <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="M92" sqref="M92"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C85" sqref="C85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1915,7 +1858,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>218</v>
+        <v>197</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1951,7 +1894,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>223</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -2936,154 +2879,148 @@
         <v>1</v>
       </c>
     </row>
-    <row r="46" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A46" s="18">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A46" s="2">
         <v>45</v>
       </c>
-      <c r="B46" s="19" t="s">
+      <c r="B46" t="s">
         <v>102</v>
       </c>
-      <c r="C46" s="19" t="s">
+      <c r="C46" t="s">
         <v>103</v>
       </c>
-      <c r="D46" s="18"/>
-      <c r="E46" s="18"/>
-      <c r="F46" s="18"/>
-      <c r="G46" s="18"/>
-      <c r="H46" s="18"/>
-      <c r="I46" s="18"/>
-      <c r="J46" s="18"/>
-      <c r="K46" s="18"/>
-      <c r="L46" s="18">
-        <v>0</v>
+      <c r="L46" s="2">
+        <v>1</v>
       </c>
       <c r="M46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A47" s="2">
         <v>46</v>
       </c>
-      <c r="B47" s="20" t="s">
+      <c r="B47" t="s">
         <v>104</v>
       </c>
-      <c r="C47" s="20" t="s">
+      <c r="C47" t="s">
         <v>105</v>
       </c>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="21"/>
-      <c r="K47" s="21"/>
-      <c r="L47" s="21">
-        <v>0</v>
+      <c r="E47" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I47" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="L47" s="2">
+        <v>3</v>
       </c>
       <c r="M47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A48" s="2">
         <v>47</v>
       </c>
-      <c r="B48" s="19" t="s">
+      <c r="B48" t="s">
         <v>106</v>
       </c>
-      <c r="C48" s="19" t="s">
+      <c r="C48" t="s">
         <v>107</v>
       </c>
-      <c r="D48" s="18"/>
-      <c r="E48" s="18"/>
-      <c r="F48" s="18"/>
-      <c r="G48" s="18"/>
-      <c r="H48" s="18"/>
-      <c r="I48" s="18"/>
-      <c r="J48" s="18"/>
-      <c r="K48" s="18"/>
-      <c r="L48" s="18">
-        <v>0</v>
+      <c r="D48" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I48" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L48" s="2">
+        <v>2</v>
       </c>
       <c r="M48">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A49" s="2">
         <v>48</v>
       </c>
-      <c r="B49" s="20" t="s">
+      <c r="B49" t="s">
         <v>108</v>
       </c>
-      <c r="C49" s="20" t="s">
+      <c r="C49" t="s">
         <v>109</v>
       </c>
-      <c r="D49" s="21"/>
-      <c r="E49" s="21"/>
-      <c r="F49" s="21"/>
-      <c r="G49" s="21"/>
-      <c r="H49" s="21"/>
-      <c r="I49" s="21"/>
-      <c r="J49" s="21"/>
-      <c r="K49" s="21"/>
-      <c r="L49" s="21">
-        <v>0</v>
+      <c r="D49" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="E49" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I49" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L49" s="2">
+        <v>3</v>
       </c>
       <c r="M49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" s="20" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A50" s="2">
         <v>49</v>
       </c>
-      <c r="B50" s="20" t="s">
+      <c r="B50" t="s">
         <v>110</v>
       </c>
-      <c r="C50" s="20" t="s">
+      <c r="C50" t="s">
         <v>111</v>
       </c>
-      <c r="D50" s="21"/>
-      <c r="E50" s="21"/>
-      <c r="F50" s="21"/>
-      <c r="G50" s="21"/>
-      <c r="H50" s="21"/>
-      <c r="I50" s="21"/>
-      <c r="J50" s="21"/>
-      <c r="K50" s="21"/>
-      <c r="L50" s="21">
-        <v>0</v>
+      <c r="D50" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E50" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I50" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L50" s="2">
+        <v>2</v>
       </c>
       <c r="M50">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="18">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A51" s="2">
         <v>50</v>
       </c>
-      <c r="B51" s="19" t="s">
+      <c r="B51" t="s">
         <v>112</v>
       </c>
-      <c r="C51" s="19" t="s">
+      <c r="C51" t="s">
         <v>113</v>
       </c>
-      <c r="D51" s="18"/>
-      <c r="E51" s="18"/>
-      <c r="F51" s="18"/>
-      <c r="G51" s="18"/>
-      <c r="H51" s="18"/>
-      <c r="I51" s="18"/>
-      <c r="J51" s="18"/>
-      <c r="K51" s="18"/>
-      <c r="L51" s="18">
-        <v>0</v>
+      <c r="D51" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E51" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I51" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L51" s="2">
+        <v>2</v>
       </c>
       <c r="M51">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:13" x14ac:dyDescent="0.25">
@@ -3096,8 +3033,17 @@
       <c r="C52" t="s">
         <v>115</v>
       </c>
+      <c r="D52" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="E52" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I52" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="L52" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M52">
         <v>0</v>
@@ -3113,11 +3059,11 @@
       <c r="C53" t="s">
         <v>117</v>
       </c>
-      <c r="E53" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I53" s="14" t="s">
+      <c r="E53" s="14" t="s">
         <v>72</v>
+      </c>
+      <c r="I53" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="L53" s="2">
         <v>3</v>
@@ -3136,17 +3082,8 @@
       <c r="C54" t="s">
         <v>119</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="E54" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="L54" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M54">
         <v>0</v>
@@ -3162,14 +3099,8 @@
       <c r="C55" t="s">
         <v>121</v>
       </c>
-      <c r="D55" s="14" t="s">
+      <c r="I55" s="14" t="s">
         <v>72</v>
-      </c>
-      <c r="E55" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I55" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="L55" s="2">
         <v>3</v>
@@ -3188,9 +3119,7 @@
       <c r="C56" t="s">
         <v>123</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="D56" s="18"/>
       <c r="E56" s="2" t="s">
         <v>75</v>
       </c>
@@ -3214,9 +3143,7 @@
       <c r="C57" t="s">
         <v>125</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="D57" s="18"/>
       <c r="E57" s="2" t="s">
         <v>75</v>
       </c>
@@ -3240,9 +3167,7 @@
       <c r="C58" t="s">
         <v>127</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="D58" s="18"/>
       <c r="E58" s="2" t="s">
         <v>75</v>
       </c>
@@ -3266,14 +3191,15 @@
       <c r="C59" t="s">
         <v>129</v>
       </c>
-      <c r="E59" s="14" t="s">
-        <v>72</v>
+      <c r="D59" s="18"/>
+      <c r="E59" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="I59" s="2" t="s">
         <v>75</v>
       </c>
       <c r="L59" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M59">
         <v>0</v>
@@ -3289,8 +3215,15 @@
       <c r="C60" t="s">
         <v>131</v>
       </c>
+      <c r="D60" s="18"/>
+      <c r="E60" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="L60" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M60">
         <v>0</v>
@@ -3306,8 +3239,12 @@
       <c r="C61" t="s">
         <v>133</v>
       </c>
-      <c r="I61" s="14" t="s">
+      <c r="D61" s="18"/>
+      <c r="E61" s="14" t="s">
         <v>72</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="L61" s="2">
         <v>3</v>
@@ -3326,15 +3263,9 @@
       <c r="C62" t="s">
         <v>135</v>
       </c>
-      <c r="D62" s="22"/>
-      <c r="E62" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I62" s="2" t="s">
-        <v>75</v>
-      </c>
+      <c r="D62" s="18"/>
       <c r="L62" s="2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="M62">
         <v>0</v>
@@ -3350,15 +3281,12 @@
       <c r="C63" t="s">
         <v>137</v>
       </c>
-      <c r="D63" s="22"/>
-      <c r="E63" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I63" s="2" t="s">
-        <v>75</v>
+      <c r="D63" s="18"/>
+      <c r="I63" s="14" t="s">
+        <v>72</v>
       </c>
       <c r="L63" s="2">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M63">
         <v>0</v>
@@ -3374,7 +3302,7 @@
       <c r="C64" t="s">
         <v>139</v>
       </c>
-      <c r="D64" s="22"/>
+      <c r="D64" s="18"/>
       <c r="E64" s="2" t="s">
         <v>75</v>
       </c>
@@ -3398,7 +3326,7 @@
       <c r="C65" t="s">
         <v>141</v>
       </c>
-      <c r="D65" s="22"/>
+      <c r="D65" s="18"/>
       <c r="E65" s="2" t="s">
         <v>75</v>
       </c>
@@ -3422,7 +3350,7 @@
       <c r="C66" t="s">
         <v>143</v>
       </c>
-      <c r="D66" s="22"/>
+      <c r="D66" s="18"/>
       <c r="E66" s="2" t="s">
         <v>75</v>
       </c>
@@ -3446,15 +3374,15 @@
       <c r="C67" t="s">
         <v>145</v>
       </c>
-      <c r="D67" s="22"/>
-      <c r="E67" s="14" t="s">
-        <v>72</v>
+      <c r="D67" s="18"/>
+      <c r="E67" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="I67" s="2" t="s">
         <v>75</v>
       </c>
       <c r="L67" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M67">
         <v>0</v>
@@ -3470,9 +3398,15 @@
       <c r="C68" t="s">
         <v>147</v>
       </c>
-      <c r="D68" s="22"/>
+      <c r="D68" s="18"/>
+      <c r="E68" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="I68" s="2" t="s">
+        <v>75</v>
+      </c>
       <c r="L68" s="2">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="M68">
         <v>0</v>
@@ -3488,9 +3422,12 @@
       <c r="C69" t="s">
         <v>149</v>
       </c>
-      <c r="D69" s="22"/>
-      <c r="I69" s="14" t="s">
+      <c r="D69" s="18"/>
+      <c r="E69" s="14" t="s">
         <v>72</v>
+      </c>
+      <c r="I69" s="2" t="s">
+        <v>75</v>
       </c>
       <c r="L69" s="2">
         <v>3</v>
@@ -3509,11 +3446,7 @@
       <c r="C70" t="s">
         <v>151</v>
       </c>
-      <c r="D70" s="22"/>
-      <c r="E70" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I70" s="2" t="s">
+      <c r="D70" s="2" t="s">
         <v>75</v>
       </c>
       <c r="L70" s="2">
@@ -3533,11 +3466,7 @@
       <c r="C71" t="s">
         <v>153</v>
       </c>
-      <c r="D71" s="22"/>
-      <c r="E71" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I71" s="2" t="s">
+      <c r="D71" s="2" t="s">
         <v>75</v>
       </c>
       <c r="L71" s="2">
@@ -3557,18 +3486,14 @@
       <c r="C72" t="s">
         <v>155</v>
       </c>
-      <c r="D72" s="22"/>
-      <c r="E72" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I72" s="2" t="s">
-        <v>75</v>
+      <c r="F72" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="L72" s="2">
         <v>2</v>
       </c>
       <c r="M72">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:13" x14ac:dyDescent="0.25">
@@ -3581,18 +3506,14 @@
       <c r="C73" t="s">
         <v>157</v>
       </c>
-      <c r="D73" s="22"/>
-      <c r="E73" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I73" s="2" t="s">
-        <v>75</v>
+      <c r="F73" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="L73" s="2">
         <v>2</v>
       </c>
       <c r="M73">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="74" spans="1:13" x14ac:dyDescent="0.25">
@@ -3605,18 +3526,14 @@
       <c r="C74" t="s">
         <v>159</v>
       </c>
-      <c r="D74" s="22"/>
-      <c r="E74" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="I74" s="2" t="s">
-        <v>75</v>
+      <c r="F74" s="2" t="s">
+        <v>29</v>
       </c>
       <c r="L74" s="2">
         <v>2</v>
       </c>
       <c r="M74">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="75" spans="1:13" x14ac:dyDescent="0.25">
@@ -3629,69 +3546,45 @@
       <c r="C75" t="s">
         <v>161</v>
       </c>
-      <c r="D75" s="22"/>
-      <c r="E75" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="I75" s="2" t="s">
-        <v>75</v>
-      </c>
       <c r="L75" s="2">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A76" s="18">
-        <v>75</v>
-      </c>
-      <c r="B76" s="19" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A76" s="2">
+        <v>75</v>
+      </c>
+      <c r="B76" t="s">
         <v>162</v>
       </c>
-      <c r="C76" s="19" t="s">
+      <c r="C76" t="s">
         <v>163</v>
       </c>
-      <c r="D76" s="18" t="s">
-        <v>75</v>
-      </c>
-      <c r="E76" s="18"/>
-      <c r="F76" s="18"/>
-      <c r="G76" s="18"/>
-      <c r="H76" s="18"/>
-      <c r="I76" s="18"/>
-      <c r="J76" s="18"/>
-      <c r="K76" s="18"/>
-      <c r="L76" s="18">
-        <v>0</v>
+      <c r="L76" s="2">
+        <v>2</v>
       </c>
       <c r="M76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A77" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A77" s="2">
         <v>76</v>
       </c>
-      <c r="B77" s="19" t="s">
+      <c r="B77" t="s">
         <v>164</v>
       </c>
-      <c r="C77" s="19" t="s">
+      <c r="C77" t="s">
         <v>165</v>
       </c>
-      <c r="D77" s="18" t="s">
-        <v>166</v>
-      </c>
-      <c r="E77" s="18"/>
-      <c r="F77" s="18"/>
-      <c r="G77" s="18"/>
-      <c r="H77" s="18"/>
-      <c r="I77" s="18"/>
-      <c r="J77" s="18"/>
-      <c r="K77" s="18"/>
-      <c r="L77" s="18">
-        <v>0</v>
+      <c r="K77" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L77" s="2">
+        <v>2</v>
       </c>
       <c r="M77">
         <v>0</v>
@@ -3702,12 +3595,12 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
+        <v>166</v>
+      </c>
+      <c r="C78" t="s">
         <v>167</v>
       </c>
-      <c r="C78" t="s">
-        <v>168</v>
-      </c>
-      <c r="D78" s="2" t="s">
+      <c r="K78" s="2" t="s">
         <v>75</v>
       </c>
       <c r="L78" s="2">
@@ -3722,12 +3615,12 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
+        <v>168</v>
+      </c>
+      <c r="C79" t="s">
         <v>169</v>
       </c>
-      <c r="C79" t="s">
-        <v>170</v>
-      </c>
-      <c r="D79" s="2" t="s">
+      <c r="J79" s="2" t="s">
         <v>75</v>
       </c>
       <c r="L79" s="2">
@@ -3742,276 +3635,72 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
+        <v>170</v>
+      </c>
+      <c r="C80" t="s">
         <v>171</v>
       </c>
-      <c r="C80" t="s">
+      <c r="J80" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="L80" s="2">
+        <v>2</v>
+      </c>
+      <c r="M80">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="81" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="16">
+        <v>80</v>
+      </c>
+      <c r="B81" s="17" t="s">
         <v>172</v>
       </c>
-      <c r="F80" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L80" s="2">
-        <v>2</v>
-      </c>
-      <c r="M80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A81" s="2">
-        <v>80</v>
-      </c>
-      <c r="B81" t="s">
+      <c r="C81" s="17" t="s">
         <v>173</v>
       </c>
-      <c r="C81" t="s">
+      <c r="D81" s="16"/>
+      <c r="E81" s="16" t="s">
         <v>174</v>
       </c>
-      <c r="F81" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L81" s="2">
-        <v>2</v>
+      <c r="F81" s="16"/>
+      <c r="G81" s="16"/>
+      <c r="H81" s="16"/>
+      <c r="I81" s="16"/>
+      <c r="J81" s="16"/>
+      <c r="K81" s="16"/>
+      <c r="L81" s="16">
+        <v>0</v>
       </c>
       <c r="M81">
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A82" s="2">
+    <row r="82" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A82" s="16">
         <v>81</v>
       </c>
-      <c r="B82" t="s">
+      <c r="B82" s="17" t="s">
         <v>175</v>
       </c>
-      <c r="C82" t="s">
+      <c r="C82" s="17" t="s">
         <v>176</v>
       </c>
-      <c r="F82" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="L82" s="2">
-        <v>2</v>
+      <c r="D82" s="16"/>
+      <c r="E82" s="16" t="s">
+        <v>174</v>
+      </c>
+      <c r="F82" s="16"/>
+      <c r="G82" s="16"/>
+      <c r="H82" s="16"/>
+      <c r="I82" s="16"/>
+      <c r="J82" s="16"/>
+      <c r="K82" s="16"/>
+      <c r="L82" s="16">
+        <v>0</v>
       </c>
       <c r="M82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A83" s="16">
-        <v>82</v>
-      </c>
-      <c r="B83" s="17" t="s">
-        <v>177</v>
-      </c>
-      <c r="C83" s="17" t="s">
-        <v>178</v>
-      </c>
-      <c r="D83" s="16"/>
-      <c r="E83" s="16"/>
-      <c r="F83" s="16"/>
-      <c r="G83" s="16"/>
-      <c r="H83" s="16"/>
-      <c r="I83" s="16"/>
-      <c r="J83" s="16"/>
-      <c r="K83" s="16"/>
-      <c r="L83" s="16">
-        <v>0</v>
-      </c>
-      <c r="M83">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="1:13" s="19" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A84" s="18">
-        <v>83</v>
-      </c>
-      <c r="B84" s="19" t="s">
-        <v>179</v>
-      </c>
-      <c r="C84" s="19" t="s">
-        <v>180</v>
-      </c>
-      <c r="D84" s="18"/>
-      <c r="E84" s="18"/>
-      <c r="F84" s="18"/>
-      <c r="G84" s="18"/>
-      <c r="H84" s="18"/>
-      <c r="I84" s="18"/>
-      <c r="J84" s="18"/>
-      <c r="K84" s="18"/>
-      <c r="L84" s="18">
-        <v>0</v>
-      </c>
-      <c r="M84">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A85" s="2">
-        <v>84</v>
-      </c>
-      <c r="B85" t="s">
-        <v>181</v>
-      </c>
-      <c r="C85" t="s">
-        <v>182</v>
-      </c>
-      <c r="L85" s="2">
-        <v>2</v>
-      </c>
-      <c r="M85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A86" s="2">
-        <v>85</v>
-      </c>
-      <c r="B86" t="s">
-        <v>183</v>
-      </c>
-      <c r="C86" t="s">
-        <v>184</v>
-      </c>
-      <c r="L86" s="2">
-        <v>2</v>
-      </c>
-      <c r="M86">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A87" s="2">
-        <v>86</v>
-      </c>
-      <c r="B87" t="s">
-        <v>185</v>
-      </c>
-      <c r="C87" t="s">
-        <v>186</v>
-      </c>
-      <c r="K87" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L87" s="2">
-        <v>2</v>
-      </c>
-      <c r="M87">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A88" s="2">
-        <v>87</v>
-      </c>
-      <c r="B88" t="s">
-        <v>187</v>
-      </c>
-      <c r="C88" t="s">
-        <v>188</v>
-      </c>
-      <c r="K88" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L88" s="2">
-        <v>2</v>
-      </c>
-      <c r="M88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A89" s="2">
-        <v>88</v>
-      </c>
-      <c r="B89" t="s">
-        <v>189</v>
-      </c>
-      <c r="C89" t="s">
-        <v>190</v>
-      </c>
-      <c r="J89" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L89" s="2">
-        <v>2</v>
-      </c>
-      <c r="M89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A90" s="2">
-        <v>89</v>
-      </c>
-      <c r="B90" t="s">
-        <v>191</v>
-      </c>
-      <c r="C90" t="s">
-        <v>192</v>
-      </c>
-      <c r="J90" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="L90" s="2">
-        <v>2</v>
-      </c>
-      <c r="M90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A91" s="16">
-        <v>90</v>
-      </c>
-      <c r="B91" s="17" t="s">
-        <v>193</v>
-      </c>
-      <c r="C91" s="17" t="s">
-        <v>194</v>
-      </c>
-      <c r="D91" s="16"/>
-      <c r="E91" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="F91" s="16"/>
-      <c r="G91" s="16"/>
-      <c r="H91" s="16"/>
-      <c r="I91" s="16"/>
-      <c r="J91" s="16"/>
-      <c r="K91" s="16"/>
-      <c r="L91" s="16">
-        <v>0</v>
-      </c>
-      <c r="M91">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="92" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A92" s="16">
-        <v>91</v>
-      </c>
-      <c r="B92" s="17" t="s">
-        <v>196</v>
-      </c>
-      <c r="C92" s="17" t="s">
-        <v>197</v>
-      </c>
-      <c r="D92" s="16"/>
-      <c r="E92" s="16" t="s">
-        <v>195</v>
-      </c>
-      <c r="F92" s="16"/>
-      <c r="G92" s="16"/>
-      <c r="H92" s="16"/>
-      <c r="I92" s="16"/>
-      <c r="J92" s="16"/>
-      <c r="K92" s="16"/>
-      <c r="L92" s="16">
-        <v>0</v>
-      </c>
-      <c r="M92">
         <v>1</v>
       </c>
     </row>
@@ -4019,4 +3708,42 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="22">
+        <v>42219</v>
+      </c>
+      <c r="B1" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>206</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Removed Hydric entries in the table
</commit_message>
<xml_diff>
--- a/Data/ResponseVariables.xlsx
+++ b/Data/ResponseVariables.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9840" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9840" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Metadata" sheetId="2" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="207">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="203">
   <si>
     <t>variable</t>
   </si>
@@ -540,21 +540,6 @@
   </si>
   <si>
     <t>Distance to nearest upstream dam</t>
-  </si>
-  <si>
-    <t>PCT_HYDRIC</t>
-  </si>
-  <si>
-    <t>Percent catchment area classified as hydric</t>
-  </si>
-  <si>
-    <t>m-calc</t>
-  </si>
-  <si>
-    <t>AREA_HYDRIC</t>
-  </si>
-  <si>
-    <t>Area (km2) catchment area classified as hydric</t>
   </si>
   <si>
     <t>Variable name used in all scripts</t>
@@ -672,6 +657,9 @@
   </si>
   <si>
     <t>Removed TotLength</t>
+  </si>
+  <si>
+    <t>Removed Hydric Layers</t>
   </si>
 </sst>
 </file>
@@ -1294,6 +1282,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="35" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -1303,7 +1292,6 @@
     <xf numFmtId="0" fontId="16" fillId="36" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1649,36 +1637,36 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="B1" s="4" t="s">
         <v>1</v>
       </c>
       <c r="C1" s="4" t="s">
-        <v>181</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>182</v>
-      </c>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
+        <v>176</v>
+      </c>
+      <c r="E1" s="22" t="s">
+        <v>177</v>
+      </c>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="C2" s="6"/>
       <c r="E2" s="12" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="F2" s="11" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="G2" s="11" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -1686,18 +1674,18 @@
         <v>0</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C3" s="6"/>
       <c r="E3" s="8" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="F3" s="10">
         <v>0</v>
       </c>
       <c r="G3" s="10">
         <f>COUNTIF(VariableRankings!L:L,F3)</f>
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -1705,11 +1693,11 @@
         <v>1</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="C4" s="6"/>
       <c r="E4" s="8" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="F4" s="10">
         <v>1</v>
@@ -1724,13 +1712,13 @@
         <v>2</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>188</v>
-      </c>
-      <c r="C5" s="19" t="s">
+        <v>183</v>
+      </c>
+      <c r="C5" s="20" t="s">
+        <v>191</v>
+      </c>
+      <c r="E5" s="8" t="s">
         <v>196</v>
-      </c>
-      <c r="E5" s="8" t="s">
-        <v>201</v>
       </c>
       <c r="F5" s="10">
         <v>2</v>
@@ -1745,11 +1733,11 @@
         <v>3</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>189</v>
-      </c>
-      <c r="C6" s="20"/>
+        <v>184</v>
+      </c>
+      <c r="C6" s="21"/>
       <c r="E6" s="8" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="F6" s="10">
         <v>3</v>
@@ -1764,64 +1752,64 @@
         <v>4</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>190</v>
-      </c>
-      <c r="C7" s="20"/>
+        <v>185</v>
+      </c>
+      <c r="C7" s="21"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>5</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>191</v>
-      </c>
-      <c r="C8" s="20"/>
+        <v>186</v>
+      </c>
+      <c r="C8" s="21"/>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>6</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>192</v>
-      </c>
-      <c r="C9" s="20"/>
+        <v>187</v>
+      </c>
+      <c r="C9" s="21"/>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>193</v>
-      </c>
-      <c r="C10" s="20"/>
+        <v>188</v>
+      </c>
+      <c r="C10" s="21"/>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
         <v>8</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>194</v>
-      </c>
-      <c r="C11" s="20"/>
+        <v>189</v>
+      </c>
+      <c r="C11" s="21"/>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>9</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>195</v>
-      </c>
-      <c r="C12" s="20"/>
+        <v>190</v>
+      </c>
+      <c r="C12" s="21"/>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>10</v>
       </c>
       <c r="B13" s="8" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
     </row>
     <row r="23" spans="3:3" x14ac:dyDescent="0.25">
@@ -1844,8 +1832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C85" sqref="C85"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C84" sqref="C84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1858,7 +1846,7 @@
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1894,7 +1882,7 @@
         <v>10</v>
       </c>
       <c r="M1" s="15" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
@@ -3630,7 +3618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A80" s="2">
         <v>79</v>
       </c>
@@ -3651,58 +3639,30 @@
       </c>
     </row>
     <row r="81" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="16">
-        <v>80</v>
-      </c>
-      <c r="B81" s="17" t="s">
-        <v>172</v>
-      </c>
-      <c r="C81" s="17" t="s">
-        <v>173</v>
-      </c>
+      <c r="A81" s="16"/>
       <c r="D81" s="16"/>
-      <c r="E81" s="16" t="s">
-        <v>174</v>
-      </c>
+      <c r="E81" s="16"/>
       <c r="F81" s="16"/>
       <c r="G81" s="16"/>
       <c r="H81" s="16"/>
       <c r="I81" s="16"/>
       <c r="J81" s="16"/>
       <c r="K81" s="16"/>
-      <c r="L81" s="16">
-        <v>0</v>
-      </c>
-      <c r="M81">
-        <v>1</v>
-      </c>
+      <c r="L81" s="16"/>
+      <c r="M81"/>
     </row>
     <row r="82" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A82" s="16">
-        <v>81</v>
-      </c>
-      <c r="B82" s="17" t="s">
-        <v>175</v>
-      </c>
-      <c r="C82" s="17" t="s">
-        <v>176</v>
-      </c>
+      <c r="A82" s="16"/>
       <c r="D82" s="16"/>
-      <c r="E82" s="16" t="s">
-        <v>174</v>
-      </c>
+      <c r="E82" s="16"/>
       <c r="F82" s="16"/>
       <c r="G82" s="16"/>
       <c r="H82" s="16"/>
       <c r="I82" s="16"/>
       <c r="J82" s="16"/>
       <c r="K82" s="16"/>
-      <c r="L82" s="16">
-        <v>0</v>
-      </c>
-      <c r="M82">
-        <v>1</v>
-      </c>
+      <c r="L82" s="16"/>
+      <c r="M82"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3712,35 +3672,40 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" s="22">
+      <c r="A1" s="19">
         <v>42219</v>
       </c>
       <c r="B1" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
-        <v>206</v>
+        <v>201</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>202</v>
       </c>
     </row>
   </sheetData>

</xml_diff>